<commit_message>
Added support for HPC Cache
</commit_message>
<xml_diff>
--- a/experimental/storage_cost_estimator/vm_storage_limits_costs.xlsx
+++ b/experimental/storage_cost_estimator/vm_storage_limits_costs.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cogarvey\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cogarvey\AppData\Local\lxss\home\linuxuser\azurehpc\experimental\storage_cost_estimator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B772349-4CF6-44F3-AB5C-0DD67B71509A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12761A8-EFB7-41C0-A79F-31B1FB525A0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{338A0779-0B5F-411A-8151-2751787F98E2}"/>
+    <workbookView xWindow="-20910" yWindow="2595" windowWidth="18945" windowHeight="27795" activeTab="2" xr2:uid="{338A0779-0B5F-411A-8151-2751787F98E2}"/>
   </bookViews>
   <sheets>
     <sheet name="VM limits" sheetId="2" r:id="rId1"/>
     <sheet name="blob" sheetId="6" r:id="rId2"/>
-    <sheet name="anf" sheetId="5" r:id="rId3"/>
-    <sheet name="Disks limits" sheetId="3" r:id="rId4"/>
+    <sheet name="hpc_cache" sheetId="7" r:id="rId3"/>
+    <sheet name="anf" sheetId="5" r:id="rId4"/>
+    <sheet name="Disks limits" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="117">
   <si>
     <t>P30</t>
   </si>
@@ -361,6 +362,33 @@
   </si>
   <si>
     <t>egress_Gbps</t>
+  </si>
+  <si>
+    <t>HPC Cache</t>
+  </si>
+  <si>
+    <t>Throughput_GBps</t>
+  </si>
+  <si>
+    <t>Capacity_small_TiB</t>
+  </si>
+  <si>
+    <t>Capacity_medium_TiB</t>
+  </si>
+  <si>
+    <t>Capacity_large_TiB</t>
+  </si>
+  <si>
+    <t>cost_small_per_month</t>
+  </si>
+  <si>
+    <t>cost_medium_per_month</t>
+  </si>
+  <si>
+    <t>cost_large_per_month</t>
+  </si>
+  <si>
+    <t>cost per Month (PAYGO)</t>
   </si>
 </sst>
 </file>
@@ -2613,8 +2641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC45FD1B-3DE4-41E2-A5E1-BB85D1E90C07}">
   <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2748,6 +2776,132 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C586F3AE-D6D1-4541-B290-DEA2F70F013E}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.59765625" customWidth="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.46484375" customWidth="1"/>
+    <col min="5" max="5" width="19.46484375" customWidth="1"/>
+    <col min="6" max="6" width="22.265625" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>4881.82</v>
+      </c>
+      <c r="F6">
+        <v>5581.5</v>
+      </c>
+      <c r="G6">
+        <v>6980.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>9763.64</v>
+      </c>
+      <c r="F7">
+        <v>11163</v>
+      </c>
+      <c r="G7">
+        <v>13961.71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>48</v>
+      </c>
+      <c r="E8">
+        <v>19527.28</v>
+      </c>
+      <c r="F8">
+        <v>22325.99</v>
+      </c>
+      <c r="G8">
+        <v>27923.32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9848403F-B453-4939-BEB6-6B3894C15104}">
   <dimension ref="A2:D8"/>
   <sheetViews>
@@ -2829,7 +2983,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6205C731-3BF1-480C-AD0B-E4E8236B2C03}">
   <dimension ref="A1:E26"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added support for Azure files and ClusterStor
</commit_message>
<xml_diff>
--- a/experimental/storage_cost_estimator/vm_storage_limits_costs.xlsx
+++ b/experimental/storage_cost_estimator/vm_storage_limits_costs.xlsx
@@ -5,19 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cogarvey\AppData\Local\lxss\home\linuxuser\azurehpc\experimental\storage_cost_estimator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cogarvey\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12761A8-EFB7-41C0-A79F-31B1FB525A0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48D7FAC-304E-4151-975F-6BFA74D14183}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20910" yWindow="2595" windowWidth="18945" windowHeight="27795" activeTab="2" xr2:uid="{338A0779-0B5F-411A-8151-2751787F98E2}"/>
+    <workbookView xWindow="-39240" yWindow="6750" windowWidth="23055" windowHeight="24930" activeTab="4" xr2:uid="{338A0779-0B5F-411A-8151-2751787F98E2}"/>
   </bookViews>
   <sheets>
     <sheet name="VM limits" sheetId="2" r:id="rId1"/>
-    <sheet name="blob" sheetId="6" r:id="rId2"/>
-    <sheet name="hpc_cache" sheetId="7" r:id="rId3"/>
-    <sheet name="anf" sheetId="5" r:id="rId4"/>
-    <sheet name="Disks limits" sheetId="3" r:id="rId5"/>
+    <sheet name="Disks limits" sheetId="3" r:id="rId2"/>
+    <sheet name="blob" sheetId="6" r:id="rId3"/>
+    <sheet name="file" sheetId="9" r:id="rId4"/>
+    <sheet name="ClusterStor" sheetId="10" r:id="rId5"/>
+    <sheet name="hpc_cache" sheetId="7" r:id="rId6"/>
+    <sheet name="ultra_disk" sheetId="8" r:id="rId7"/>
+    <sheet name="anf" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="144">
   <si>
     <t>P30</t>
   </si>
@@ -388,7 +391,88 @@
     <t>cost_large_per_month</t>
   </si>
   <si>
-    <t>cost per Month (PAYGO)</t>
+    <t>Ultra Disks</t>
+  </si>
+  <si>
+    <t>Min_disk_size_GiB</t>
+  </si>
+  <si>
+    <t>Max_disk_size_GiB</t>
+  </si>
+  <si>
+    <t>Max_throughput_per_disk_MBps</t>
+  </si>
+  <si>
+    <t>Throughput_per_GiB_MBps</t>
+  </si>
+  <si>
+    <t>Throughput_per_IOPS_KiBps</t>
+  </si>
+  <si>
+    <t>IOPS_per_GiB</t>
+  </si>
+  <si>
+    <t>Disk_capacity_cost_per_month_per_GiB</t>
+  </si>
+  <si>
+    <t>Cost_per_month_per_IOPS</t>
+  </si>
+  <si>
+    <t>Cost_per_month_per_throughput_MBps</t>
+  </si>
+  <si>
+    <t>Max_IOPS</t>
+  </si>
+  <si>
+    <t>Azure Files</t>
+  </si>
+  <si>
+    <t>egress_MiBps_per_GiB</t>
+  </si>
+  <si>
+    <t>ingress_MiBps_per_GiB</t>
+  </si>
+  <si>
+    <t>cost_per_GiB</t>
+  </si>
+  <si>
+    <t>Max_size_TiB</t>
+  </si>
+  <si>
+    <t>IOPS_baseline</t>
+  </si>
+  <si>
+    <t>ingress_MiBps_baseline</t>
+  </si>
+  <si>
+    <t>egress_MiBps_baseline</t>
+  </si>
+  <si>
+    <t>Max_egress_MiBps</t>
+  </si>
+  <si>
+    <t>Max_ingress_MiBps</t>
+  </si>
+  <si>
+    <t>transaction optimized</t>
+  </si>
+  <si>
+    <t>ClusterStor</t>
+  </si>
+  <si>
+    <t>3 year cost</t>
+  </si>
+  <si>
+    <t>Monthly_cost</t>
+  </si>
+  <si>
+    <t>Read_GBps</t>
+  </si>
+  <si>
+    <t>Write_GBps</t>
+  </si>
+  <si>
+    <t>Capacity_PiB</t>
   </si>
 </sst>
 </file>
@@ -748,7 +832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F001577-E445-4318-A48D-6522BC2A4F70}">
   <dimension ref="A2:N55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2638,11 +2722,415 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6205C731-3BF1-480C-AD0B-E4E8236B2C03}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="14.1328125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <v>62</v>
+      </c>
+      <c r="D6">
+        <v>2300</v>
+      </c>
+      <c r="E6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>116.75</v>
+      </c>
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>223.75</v>
+      </c>
+      <c r="D8">
+        <v>7500</v>
+      </c>
+      <c r="E8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>428</v>
+      </c>
+      <c r="D9">
+        <v>7500</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>817.16</v>
+      </c>
+      <c r="D10">
+        <v>16000</v>
+      </c>
+      <c r="E10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>1556.5</v>
+      </c>
+      <c r="D11">
+        <v>18000</v>
+      </c>
+      <c r="E11">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>3113</v>
+      </c>
+      <c r="D12">
+        <v>20000</v>
+      </c>
+      <c r="E12">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+      <c r="C13">
+        <v>38.4</v>
+      </c>
+      <c r="D13">
+        <v>500</v>
+      </c>
+      <c r="E13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>76.8</v>
+      </c>
+      <c r="D14">
+        <v>500</v>
+      </c>
+      <c r="E14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>153.6</v>
+      </c>
+      <c r="D15">
+        <v>500</v>
+      </c>
+      <c r="E15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>307.2</v>
+      </c>
+      <c r="D16">
+        <v>500</v>
+      </c>
+      <c r="E16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>614.20000000000005</v>
+      </c>
+      <c r="D17">
+        <v>2000</v>
+      </c>
+      <c r="E17">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>1228.8</v>
+      </c>
+      <c r="D18">
+        <v>4000</v>
+      </c>
+      <c r="E18">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>2457.6</v>
+      </c>
+      <c r="D19">
+        <v>6000</v>
+      </c>
+      <c r="E19">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>0.5</v>
+      </c>
+      <c r="C20">
+        <v>21.76</v>
+      </c>
+      <c r="D20">
+        <v>500</v>
+      </c>
+      <c r="E20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>40.96</v>
+      </c>
+      <c r="D21">
+        <v>500</v>
+      </c>
+      <c r="E21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>81.92</v>
+      </c>
+      <c r="D22">
+        <v>500</v>
+      </c>
+      <c r="E22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>163.84</v>
+      </c>
+      <c r="D23">
+        <v>500</v>
+      </c>
+      <c r="E23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>327.68</v>
+      </c>
+      <c r="D24">
+        <v>1300</v>
+      </c>
+      <c r="E24">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>655.36</v>
+      </c>
+      <c r="D25">
+        <v>2000</v>
+      </c>
+      <c r="E25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>1310.72</v>
+      </c>
+      <c r="D26">
+        <v>2000</v>
+      </c>
+      <c r="E26">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC45FD1B-3DE4-41E2-A5E1-BB85D1E90C07}">
-  <dimension ref="A2:F12"/>
+  <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2655,22 +3143,22 @@
     <col min="6" max="6" width="21.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -2689,8 +3177,11 @@
       <c r="F8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -2709,8 +3200,11 @@
       <c r="F9">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G9">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -2729,8 +3223,11 @@
       <c r="F10">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G10">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -2749,8 +3246,11 @@
       <c r="F11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G11">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -2769,131 +3269,8 @@
       <c r="F12">
         <v>2E-3</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C586F3AE-D6D1-4541-B290-DEA2F70F013E}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="15.59765625" customWidth="1"/>
-    <col min="2" max="2" width="16.796875" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.46484375" customWidth="1"/>
-    <col min="5" max="5" width="19.46484375" customWidth="1"/>
-    <col min="6" max="6" width="22.265625" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>4881.82</v>
-      </c>
-      <c r="F6">
-        <v>5581.5</v>
-      </c>
-      <c r="G6">
-        <v>6980.86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>24</v>
-      </c>
-      <c r="E7">
-        <v>9763.64</v>
-      </c>
-      <c r="F7">
-        <v>11163</v>
-      </c>
-      <c r="G7">
-        <v>13961.71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>24</v>
-      </c>
-      <c r="D8">
-        <v>48</v>
-      </c>
-      <c r="E8">
-        <v>19527.28</v>
-      </c>
-      <c r="F8">
-        <v>22325.99</v>
-      </c>
-      <c r="G8">
-        <v>27923.32</v>
+      <c r="G12">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>
@@ -2902,10 +3279,585 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71C063B-B741-4C7E-8017-0619ED5B702D}">
+  <dimension ref="A2:N12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.9296875" customWidth="1"/>
+    <col min="3" max="3" width="21.73046875" customWidth="1"/>
+    <col min="4" max="4" width="13.73046875" customWidth="1"/>
+    <col min="5" max="5" width="21.73046875" customWidth="1"/>
+    <col min="6" max="6" width="21.06640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.265625" customWidth="1"/>
+    <col min="9" max="9" width="13.59765625" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="21.73046875" customWidth="1"/>
+    <col min="12" max="12" width="16.53125" customWidth="1"/>
+    <col min="13" max="13" width="16.3984375" customWidth="1"/>
+    <col min="14" max="14" width="16.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" t="s">
+        <v>131</v>
+      </c>
+      <c r="I8" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K8" t="s">
+        <v>133</v>
+      </c>
+      <c r="L8" t="s">
+        <v>134</v>
+      </c>
+      <c r="M8" t="s">
+        <v>135</v>
+      </c>
+      <c r="N8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9">
+        <v>0.06</v>
+      </c>
+      <c r="C9">
+        <v>0.04</v>
+      </c>
+      <c r="D9">
+        <v>0.192</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>100000</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>400</v>
+      </c>
+      <c r="K9">
+        <v>40</v>
+      </c>
+      <c r="L9">
+        <v>60</v>
+      </c>
+      <c r="M9">
+        <v>6204</v>
+      </c>
+      <c r="N9">
+        <v>4136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="C10">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="D10">
+        <v>0.06</v>
+      </c>
+      <c r="E10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F10">
+        <v>1.5E-3</v>
+      </c>
+      <c r="G10">
+        <v>10000</v>
+      </c>
+      <c r="H10">
+        <v>100</v>
+      </c>
+      <c r="I10">
+        <v>0.1</v>
+      </c>
+      <c r="J10">
+        <v>40</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>6</v>
+      </c>
+      <c r="M10">
+        <v>300</v>
+      </c>
+      <c r="N10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="C11">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="D11">
+        <v>2.76E-2</v>
+      </c>
+      <c r="E11">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="F11">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="G11">
+        <v>10000</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="I11">
+        <v>0.1</v>
+      </c>
+      <c r="J11">
+        <v>40</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="M11">
+        <v>300</v>
+      </c>
+      <c r="N11">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="C12">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="D12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.13</v>
+      </c>
+      <c r="F12">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G12">
+        <v>10000</v>
+      </c>
+      <c r="H12">
+        <v>100</v>
+      </c>
+      <c r="I12">
+        <v>0.1</v>
+      </c>
+      <c r="J12">
+        <v>40</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <v>300</v>
+      </c>
+      <c r="N12">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F239E3-A366-4F2A-95CD-84604D27B2B6}">
+  <dimension ref="A2:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.86328125" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="12.9296875" customWidth="1"/>
+    <col min="5" max="5" width="14.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1500000</v>
+      </c>
+      <c r="C8">
+        <f>B8/36</f>
+        <v>41666.666666666664</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <f>B8*3</f>
+        <v>4500000</v>
+      </c>
+      <c r="C9">
+        <f>B9/36</f>
+        <v>125000</v>
+      </c>
+      <c r="D9">
+        <f>D8*3</f>
+        <v>150</v>
+      </c>
+      <c r="E9">
+        <f>E8*3</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <f>B8*9</f>
+        <v>13500000</v>
+      </c>
+      <c r="C10">
+        <f>B10/36</f>
+        <v>375000</v>
+      </c>
+      <c r="D10">
+        <f>D8*9</f>
+        <v>450</v>
+      </c>
+      <c r="E10">
+        <f>E8*9</f>
+        <v>450</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EDE043C-47B1-4032-9BBB-273FB06C87F1}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.1328125" customWidth="1"/>
+    <col min="2" max="2" width="18.265625" customWidth="1"/>
+    <col min="3" max="3" width="16.265625" customWidth="1"/>
+    <col min="4" max="4" width="17.19921875" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="24.1328125" customWidth="1"/>
+    <col min="7" max="7" width="20.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>4881.82</v>
+      </c>
+      <c r="F6">
+        <v>5581.5</v>
+      </c>
+      <c r="G6">
+        <v>6980.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>9763.64</v>
+      </c>
+      <c r="F7">
+        <v>11163</v>
+      </c>
+      <c r="G7">
+        <v>13961.71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>48</v>
+      </c>
+      <c r="E8">
+        <v>19527.28</v>
+      </c>
+      <c r="F8">
+        <v>22325.99</v>
+      </c>
+      <c r="G8">
+        <v>27923.32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC686640-D7FD-4250-BFEC-140FE03FF552}">
+  <dimension ref="A2:I6"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="19.19921875" customWidth="1"/>
+    <col min="3" max="3" width="30.265625" customWidth="1"/>
+    <col min="4" max="4" width="24.3984375" customWidth="1"/>
+    <col min="5" max="5" width="25.06640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="36.1328125" customWidth="1"/>
+    <col min="8" max="8" width="24.3984375" customWidth="1"/>
+    <col min="9" max="9" width="35.19921875" customWidth="1"/>
+    <col min="10" max="10" width="20.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>65536</v>
+      </c>
+      <c r="C6">
+        <v>2000</v>
+      </c>
+      <c r="D6">
+        <v>75</v>
+      </c>
+      <c r="E6">
+        <v>256</v>
+      </c>
+      <c r="F6">
+        <v>300</v>
+      </c>
+      <c r="G6">
+        <v>0.15</v>
+      </c>
+      <c r="H6">
+        <v>0.06</v>
+      </c>
+      <c r="I6">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9848403F-B453-4939-BEB6-6B3894C15104}">
   <dimension ref="A2:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -2983,410 +3935,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6205C731-3BF1-480C-AD0B-E4E8236B2C03}">
-  <dimension ref="A1:E26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="3" max="3" width="14.1328125" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.3984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6">
-        <v>0.5</v>
-      </c>
-      <c r="C6">
-        <v>62</v>
-      </c>
-      <c r="D6">
-        <v>2300</v>
-      </c>
-      <c r="E6">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>116.75</v>
-      </c>
-      <c r="D7">
-        <v>5000</v>
-      </c>
-      <c r="E7">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>223.75</v>
-      </c>
-      <c r="D8">
-        <v>7500</v>
-      </c>
-      <c r="E8">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>428</v>
-      </c>
-      <c r="D9">
-        <v>7500</v>
-      </c>
-      <c r="E9">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>817.16</v>
-      </c>
-      <c r="D10">
-        <v>16000</v>
-      </c>
-      <c r="E10">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>1556.5</v>
-      </c>
-      <c r="D11">
-        <v>18000</v>
-      </c>
-      <c r="E11">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12">
-        <v>32</v>
-      </c>
-      <c r="C12">
-        <v>3113</v>
-      </c>
-      <c r="D12">
-        <v>20000</v>
-      </c>
-      <c r="E12">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13">
-        <v>0.5</v>
-      </c>
-      <c r="C13">
-        <v>38.4</v>
-      </c>
-      <c r="D13">
-        <v>500</v>
-      </c>
-      <c r="E13">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>76.8</v>
-      </c>
-      <c r="D14">
-        <v>500</v>
-      </c>
-      <c r="E14">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>153.6</v>
-      </c>
-      <c r="D15">
-        <v>500</v>
-      </c>
-      <c r="E15">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>307.2</v>
-      </c>
-      <c r="D16">
-        <v>500</v>
-      </c>
-      <c r="E16">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>614.20000000000005</v>
-      </c>
-      <c r="D17">
-        <v>2000</v>
-      </c>
-      <c r="E17">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18">
-        <v>16</v>
-      </c>
-      <c r="C18">
-        <v>1228.8</v>
-      </c>
-      <c r="D18">
-        <v>4000</v>
-      </c>
-      <c r="E18">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19">
-        <v>32</v>
-      </c>
-      <c r="C19">
-        <v>2457.6</v>
-      </c>
-      <c r="D19">
-        <v>6000</v>
-      </c>
-      <c r="E19">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20">
-        <v>0.5</v>
-      </c>
-      <c r="C20">
-        <v>21.76</v>
-      </c>
-      <c r="D20">
-        <v>500</v>
-      </c>
-      <c r="E20">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>40.96</v>
-      </c>
-      <c r="D21">
-        <v>500</v>
-      </c>
-      <c r="E21">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>81.92</v>
-      </c>
-      <c r="D22">
-        <v>500</v>
-      </c>
-      <c r="E22">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23">
-        <v>163.84</v>
-      </c>
-      <c r="D23">
-        <v>500</v>
-      </c>
-      <c r="E23">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24">
-        <v>8</v>
-      </c>
-      <c r="C24">
-        <v>327.68</v>
-      </c>
-      <c r="D24">
-        <v>1300</v>
-      </c>
-      <c r="E24">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25">
-        <v>16</v>
-      </c>
-      <c r="C25">
-        <v>655.36</v>
-      </c>
-      <c r="D25">
-        <v>2000</v>
-      </c>
-      <c r="E25">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26">
-        <v>32</v>
-      </c>
-      <c r="C26">
-        <v>1310.72</v>
-      </c>
-      <c r="D26">
-        <v>2000</v>
-      </c>
-      <c r="E26">
-        <v>500</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>